<commit_message>
Complete bill of materials for MAX15046B_5V circuit. As well as updates to the schematic and PCB itself.
</commit_message>
<xml_diff>
--- a/Misc/gEDA_Projects/MAXIM15046B_Layout/BOM_5V_10A.xlsx
+++ b/Misc/gEDA_Projects/MAXIM15046B_Layout/BOM_5V_10A.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
   <si>
     <t>Ref</t>
   </si>
@@ -62,7 +62,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="10"/>
@@ -195,6 +194,18 @@
   </si>
   <si>
     <t>C119</t>
+  </si>
+  <si>
+    <t>CON101</t>
+  </si>
+  <si>
+    <t>MOLEX1720640006</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings Mega-Fit RA Hdr Assy 6 ckt 15u" Au</t>
   </si>
   <si>
     <t>D101</t>
@@ -325,10 +336,9 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -349,33 +359,22 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <color rgb="000000FF"/>
       <sz val="10"/>
       <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="000000FF"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="000000FF"/>
-      <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -460,31 +459,32 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="2" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="2" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -502,48 +502,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:32"/>
+  <dimension ref="1:33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="false" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A18" activeCellId="0" pane="topLeft" sqref="18:18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="false" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C9" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E18" activeCellId="0" pane="topLeft" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.13725490196079"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.48627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="84.7254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5098039215686"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.16470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.50588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.8039215686274"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1019607843137"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.1450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.0078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5647058823529"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="1" s="4">
-      <c r="A1" s="2" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="1" s="6">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AMJ1" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="2">
+      <c r="AMJ1" s="8"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -553,14 +553,14 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -570,14 +570,14 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -587,14 +587,14 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -604,14 +604,14 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -621,14 +621,14 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -638,14 +638,14 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -655,14 +655,14 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -672,14 +672,14 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -689,14 +689,14 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -706,14 +706,14 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -723,14 +723,14 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -740,14 +740,14 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -757,14 +757,14 @@
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="0" t="s">
@@ -774,14 +774,14 @@
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D16" s="0" t="s">
@@ -798,7 +798,7 @@
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -808,246 +808,263 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.55" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="13"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="19">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.55" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="20">
+      <c r="F19" s="13"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="21">
+      <c r="E20" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>68</v>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="13"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="22">
+        <v>70</v>
+      </c>
+      <c r="E21" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.65" outlineLevel="0" r="23">
+      <c r="E22" s="13"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="24">
+        <v>75</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.65" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="25">
+      <c r="E24" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>78</v>
+      <c r="C25" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="26">
+        <v>75</v>
+      </c>
+      <c r="E25" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>81</v>
+      <c r="C26" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="27">
+        <v>75</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>83</v>
+      <c r="C27" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="28">
+        <v>75</v>
+      </c>
+      <c r="E27" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>85</v>
+      <c r="C28" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="29">
+        <v>75</v>
+      </c>
+      <c r="E28" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>87</v>
+      <c r="C29" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="30">
+        <v>75</v>
+      </c>
+      <c r="E29" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>89</v>
+      <c r="C30" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="F30" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="31">
+        <v>75</v>
+      </c>
+      <c r="E30" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>92</v>
+      <c r="C31" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="32">
+        <v>75</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>94</v>
+      <c r="C32" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" s="8"/>
+        <v>75</v>
+      </c>
+      <c r="E32" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="33">
+      <c r="A33" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1067,21 +1084,22 @@
     <hyperlink display="GRM155R71H182KA01" ref="C15" r:id="rId14"/>
     <hyperlink display="GRM155R71H681KA01D" ref="C16" r:id="rId15"/>
     <hyperlink display="GRM155R71C104KA88D" ref="C17" r:id="rId16"/>
-    <hyperlink display="ZHCS506" ref="C18" r:id="rId17"/>
-    <hyperlink display="DO5040H-392MLB" ref="C19" r:id="rId18"/>
-    <hyperlink display="SI7850DP-T1-E3" ref="C20" r:id="rId19"/>
-    <hyperlink display="Si7460DP-T1-E3" ref="C21" r:id="rId20"/>
-    <hyperlink display="CRCW040210R0FKED" ref="C22" r:id="rId21"/>
-    <hyperlink display="CRCW040251K1FKED" ref="C23" r:id="rId22"/>
-    <hyperlink display="CRCW04022R21FKED" ref="C24" r:id="rId23"/>
-    <hyperlink display="CRCW120610R0FKEA" ref="C25" r:id="rId24"/>
-    <hyperlink display="CRCW040230K9FKED" ref="C26" r:id="rId25"/>
-    <hyperlink display="CRCW040222K6FKED" ref="C27" r:id="rId26"/>
-    <hyperlink display="CRCW04021K33FKED" ref="C28" r:id="rId27"/>
-    <hyperlink display="CRCW040248K7FKED" ref="C29" r:id="rId28"/>
-    <hyperlink display="CRCW04026K49FKED" ref="C30" r:id="rId29"/>
-    <hyperlink display="CRCW040247K5FKED" ref="C31" r:id="rId30"/>
-    <hyperlink display="CRCW080549R9FKEA" ref="C32" r:id="rId31"/>
+    <hyperlink display="MOLEX1720640006" ref="C18" r:id="rId17"/>
+    <hyperlink display="ZHCS506" ref="C19" r:id="rId18"/>
+    <hyperlink display="DO5040H-392MLB" ref="C20" r:id="rId19"/>
+    <hyperlink display="SI7850DP-T1-E3" ref="C21" r:id="rId20"/>
+    <hyperlink display="Si7460DP-T1-E3" ref="C22" r:id="rId21"/>
+    <hyperlink display="CRCW040210R0FKED" ref="C23" r:id="rId22"/>
+    <hyperlink display="CRCW040251K1FKED" ref="C24" r:id="rId23"/>
+    <hyperlink display="CRCW04022R21FKED" ref="C25" r:id="rId24"/>
+    <hyperlink display="CRCW120610R0FKEA" ref="C26" r:id="rId25"/>
+    <hyperlink display="CRCW040230K9FKED" ref="C27" r:id="rId26"/>
+    <hyperlink display="CRCW040222K6FKED" ref="C28" r:id="rId27"/>
+    <hyperlink display="CRCW04021K33FKED" ref="C29" r:id="rId28"/>
+    <hyperlink display="CRCW040248K7FKED" ref="C30" r:id="rId29"/>
+    <hyperlink display="CRCW04026K49FKED" ref="C31" r:id="rId30"/>
+    <hyperlink display="CRCW040247K5FKED" ref="C32" r:id="rId31"/>
+    <hyperlink display="CRCW080549R9FKEA" ref="C33" r:id="rId32"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>